<commit_message>
Iniital analysis of Crizer data complete
</commit_message>
<xml_diff>
--- a/working/CrizerPFAS/CrizerChemIDs.xlsx
+++ b/working/CrizerPFAS/CrizerChemIDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\CrizerPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{624A5724-3477-453F-855E-CEC6C2CB59BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A2F14E-C779-49FD-B433-6A0A94CE26AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29970" yWindow="2850" windowWidth="27630" windowHeight="11715" xr2:uid="{819F4BB0-2119-468F-947F-0171544AB1A3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{819F4BB0-2119-468F-947F-0171544AB1A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="88">
   <si>
     <t>Chemical</t>
   </si>
@@ -48,19 +48,276 @@
   </si>
   <si>
     <t>DTXSID20874028</t>
+  </si>
+  <si>
+    <t>8:2_Fluoroteleomer_Sulfonic_Acid</t>
+  </si>
+  <si>
+    <t>DTXSID00192353</t>
+  </si>
+  <si>
+    <t>3:3_Fluorotelomer_carboxylic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID00379268</t>
+  </si>
+  <si>
+    <t>DTXSID00880026</t>
+  </si>
+  <si>
+    <t>Potassium_perfluorooctanoate</t>
+  </si>
+  <si>
+    <t>N-Ethylperfluorooctanesulfonamide</t>
+  </si>
+  <si>
+    <t>DTXSID1032646</t>
+  </si>
+  <si>
+    <t>Perfluoroheptanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID1037303</t>
+  </si>
+  <si>
+    <t>N-Methylperfluorooctanesulfonamide</t>
+  </si>
+  <si>
+    <t>DTXSID1067629</t>
+  </si>
+  <si>
+    <t>2-(Perfluorohexyl)ethylphosphonic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID20179883</t>
+  </si>
+  <si>
+    <t>3,3-Bis(trifluoromethyl)-2-propenoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID30170109</t>
+  </si>
+  <si>
+    <t>Perfluorodecanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID3031860</t>
+  </si>
+  <si>
+    <t>Perfluorohexanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID3031862</t>
+  </si>
+  <si>
+    <t>Perfluorooctanesulfonic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID3031864</t>
+  </si>
+  <si>
+    <t>Potassium_perfluorobutanesulfonate</t>
+  </si>
+  <si>
+    <t>DTXSID3037707</t>
+  </si>
+  <si>
+    <t>Potassium_Pefluorohexanesulfate</t>
+  </si>
+  <si>
+    <t>DTXSID3037709</t>
+  </si>
+  <si>
+    <t>Perfluoro-3,6-dioxaheptanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID30382063</t>
+  </si>
+  <si>
+    <t>Perfluorotetradecanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID3059921</t>
+  </si>
+  <si>
+    <t>4:2_Fluorotelomer_sulfonic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID30891564</t>
+  </si>
+  <si>
+    <t>3-(Perfluoroisopropyl)-2-propenoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID40380257</t>
+  </si>
+  <si>
+    <t>Perfluorobutanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID4059916</t>
+  </si>
+  <si>
+    <t>Sodium_perfluorooctanoate</t>
+  </si>
+  <si>
+    <t>DTXSID40880025</t>
+  </si>
+  <si>
+    <t>Perfluorobutanesulfonic_acid</t>
+  </si>
+  <si>
+    <t>Perfluorohexanesulfonamide</t>
+  </si>
+  <si>
+    <t>DTXSID5030030</t>
+  </si>
+  <si>
+    <t>DTXSID50469320</t>
+  </si>
+  <si>
+    <t>11-H-Perfluoroundecanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID5061954</t>
+  </si>
+  <si>
+    <t>4H-Perfluorobutanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID50892417</t>
+  </si>
+  <si>
+    <t>2,2,2-Trifluoroethyl_perfluorobutanesulfonate</t>
+  </si>
+  <si>
+    <t>DTXSID60380390</t>
+  </si>
+  <si>
+    <t>Perfluoro(4-methoxybutanoic)_acid</t>
+  </si>
+  <si>
+    <t>DTXSID60500450</t>
+  </si>
+  <si>
+    <t>Perfluoropentanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID6062599</t>
+  </si>
+  <si>
+    <t>Perfluoro-4-isopropoxybutanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID60663110</t>
+  </si>
+  <si>
+    <t>6:2_Fluorotelomer_sulfonic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID6067331</t>
+  </si>
+  <si>
+    <t>Sodium_perfluorodecanesulfonate</t>
+  </si>
+  <si>
+    <t>DTXSID60892443</t>
+  </si>
+  <si>
+    <t>Perfluoro-3-methoxypropanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID70191136</t>
+  </si>
+  <si>
+    <t>Perfluorohexanesulfonic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID7040150</t>
+  </si>
+  <si>
+    <t>Perfluorooctanesulfonate</t>
+  </si>
+  <si>
+    <t>DTXSID80108992</t>
+  </si>
+  <si>
+    <t>Perfluorononanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID8031863</t>
+  </si>
+  <si>
+    <t>Perfluorooctanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID8031865</t>
+  </si>
+  <si>
+    <t>Potassium_perfluorooctanesulfonate</t>
+  </si>
+  <si>
+    <t>DTXSID8037706</t>
+  </si>
+  <si>
+    <t>Ammonium_perfluorooctanoate</t>
+  </si>
+  <si>
+    <t>DTXSID8037708</t>
+  </si>
+  <si>
+    <t>Perfluoroundecanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID8047553</t>
+  </si>
+  <si>
+    <t>Perfluorooctanesulfonamido_ammonium_iodide</t>
+  </si>
+  <si>
+    <t>DTXSID8051419</t>
+  </si>
+  <si>
+    <t>Perfluoroheptanesulfonic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID8059920</t>
+  </si>
+  <si>
+    <t>Perfluoropropanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID8059970</t>
+  </si>
+  <si>
+    <t>Perfluoro-1-octanesulfonyl_chloride</t>
+  </si>
+  <si>
+    <t>DTXSID90315130</t>
+  </si>
+  <si>
+    <t>Perfluorotridecanoic_acid</t>
+  </si>
+  <si>
+    <t>DTXSID90868151</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -83,13 +340,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <color auto="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -100,6 +381,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{61DDEC30-F9B7-48F5-A8B3-DBABB6D1E149}" name="Table1" displayName="Table1" ref="A1:B44" totalsRowShown="0">
+  <autoFilter ref="A1:B44" xr:uid="{61DDEC30-F9B7-48F5-A8B3-DBABB6D1E149}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CF27F945-8CE4-4AC2-B5C3-1FDA67ACBD79}" name="Chemical" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{7AA6CD87-74DC-4D34-B235-20B5844CCA97}" name="DTXSID"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -399,13 +691,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDE8F23D-687E-440F-B10F-6183CD66E1B7}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
@@ -423,7 +719,347 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" t="s">
+        <v>87</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>